<commit_message>
actions working mostly, rewards for probabilistic actions are distributed with +-30% non-unfiformly
</commit_message>
<xml_diff>
--- a/balancing.xlsx
+++ b/balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\wanted-idle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2E136-9D41-4D0C-946D-35322370F714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B4B54C-7D0F-4C98-93E5-27AEAC2C6A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19110" yWindow="8655" windowWidth="38700" windowHeight="15435" xr2:uid="{AF0AD4B1-6F56-4A44-BD00-A6D72CE51D30}"/>
+    <workbookView xWindow="6600" yWindow="2370" windowWidth="38700" windowHeight="15435" xr2:uid="{AF0AD4B1-6F56-4A44-BD00-A6D72CE51D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>v</t>
   </si>
@@ -118,6 +120,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -477,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6154F62F-A163-4FC9-8540-1F7086C4AFC0}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -489,7 +494,7 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -511,8 +516,14 @@
       <c r="H1">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -523,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <f>C2*$H$2/B2</f>
+        <f t="shared" ref="D2:D7" si="0">C2*$H$2/B2</f>
         <v>30</v>
       </c>
       <c r="E2" t="s">
@@ -539,8 +550,15 @@
         <f>60*H1</f>
         <v>1200</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> 924*POWER(K2,13) - 6006 * POWER(K2,12) + 16380 * POWER(K2,11) - 24024 * POWER(K2,10)  + 20020 * POWER(K2,9) - 9009 * POWER(K2,8) + 1716 * POWER(K2,7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -551,7 +569,7 @@
         <v>1.2</v>
       </c>
       <c r="D3">
-        <f>C3*$H$2/B3</f>
+        <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
       <c r="E3" t="s">
@@ -560,8 +578,15 @@
       <c r="F3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L12" si="1" xml:space="preserve"> 924*POWER(K3,13) - 6006 * POWER(K3,12) + 16380 * POWER(K3,11) - 24024 * POWER(K3,10)  + 20020 * POWER(K3,9) - 9009 * POWER(K3,8) + 1716 * POWER(K3,7)</f>
+        <v>9.9285486400000066E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -572,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f>C4*$H$2/B4</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="E4" t="s">
@@ -581,8 +606,15 @@
       <c r="F4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>7.0035611648000037E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -593,7 +625,7 @@
         <v>1.2</v>
       </c>
       <c r="D5">
-        <f>C5*$H$2/B5</f>
+        <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
       <c r="E5" t="s">
@@ -602,8 +634,15 @@
       <c r="F5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5">
+        <v>0.3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>6.237521179919997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -614,7 +653,7 @@
         <v>0.5</v>
       </c>
       <c r="D6">
-        <f>C6*$H$2/B6</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E6" t="s">
@@ -624,8 +663,15 @@
         <v>23</v>
       </c>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6">
+        <v>0.4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>0.22884395253759982</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -636,7 +682,7 @@
         <v>0.5</v>
       </c>
       <c r="D7">
-        <f>C7*$H$2/B7</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="E7" t="s">
@@ -646,8 +692,15 @@
         <v>23</v>
       </c>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7">
+        <v>0.5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -665,8 +718,15 @@
         <v>23</v>
       </c>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8">
+        <v>0.6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0.77115604746240507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -677,15 +737,22 @@
         <v>1.8</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D22" si="0">B9*C9*$H$2</f>
+        <f t="shared" ref="D9:D22" si="2">B9*C9*$H$2</f>
         <v>18.468</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="K9">
+        <v>0.7</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>0.93762478820084993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -696,15 +763,22 @@
         <v>1.44</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14.428800000000001</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="K10">
+        <v>0.8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>0.99299643883495037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -715,15 +789,22 @@
         <v>2.37</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>23.463000000000001</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="K11">
+        <v>0.9</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>0.99990071451395579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -734,15 +815,22 @@
         <v>1.18</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.9827999999999992</v>
       </c>
       <c r="F12" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -753,7 +841,7 @@
         <v>3.75</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>28.8</v>
       </c>
       <c r="F13" t="s">
@@ -761,7 +849,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -772,7 +860,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>24.0642</v>
       </c>
       <c r="F14" t="s">
@@ -780,7 +868,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -791,7 +879,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14.415599999999998</v>
       </c>
       <c r="F15" t="s">
@@ -799,7 +887,7 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -810,7 +898,7 @@
         <v>11.1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>25.973999999999997</v>
       </c>
       <c r="F16" t="s">
@@ -829,7 +917,7 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30.06</v>
       </c>
       <c r="F17" t="s">
@@ -848,7 +936,7 @@
         <v>32.11</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>26.9724</v>
       </c>
       <c r="F18" t="s">
@@ -867,7 +955,7 @@
         <v>16.84</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19.197599999999998</v>
       </c>
       <c r="F19" t="s">
@@ -886,7 +974,7 @@
         <v>44.44</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>29.863679999999995</v>
       </c>
       <c r="F20" t="s">
@@ -904,7 +992,7 @@
         <v>50</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="F21" t="s">
@@ -922,7 +1010,7 @@
         <v>300</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>14.4</v>
       </c>
       <c r="F22" t="s">

</xml_diff>

<commit_message>
First version with ends.
</commit_message>
<xml_diff>
--- a/balancing.xlsx
+++ b/balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\wanted-idle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C454BE-B7F3-41F3-853B-338DF82478FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A969EC-228B-4286-B177-9803A0731017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2340" yWindow="1770" windowWidth="38700" windowHeight="15435" xr2:uid="{AF0AD4B1-6F56-4A44-BD00-A6D72CE51D30}"/>
+    <workbookView xWindow="5325" yWindow="2670" windowWidth="38700" windowHeight="15435" xr2:uid="{AF0AD4B1-6F56-4A44-BD00-A6D72CE51D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>v</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>min bis a</t>
+  </si>
+  <si>
+    <t>reached</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -166,11 +175,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -485,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6154F62F-A163-4FC9-8540-1F7086C4AFC0}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -497,7 +508,7 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -522,8 +533,20 @@
       <c r="L1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1">
+        <v>5000</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -554,8 +577,23 @@
         <f xml:space="preserve"> 924*POWER(K2,13) - 6006 * POWER(K2,12) + 16380 * POWER(K2,11) - 24024 * POWER(K2,10)  + 20020 * POWER(K2,9) - 9009 * POWER(K2,8) + 1716 * POWER(K2,7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="O2">
+        <v>10</v>
+      </c>
+      <c r="P2" s="2">
+        <f>$P$1/O2*$H$2</f>
+        <v>300000</v>
+      </c>
+      <c r="Q2" s="2">
+        <f>$P$1/O2</f>
+        <v>500</v>
+      </c>
+      <c r="R2" s="3">
+        <f>Q2/60</f>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -579,8 +617,23 @@
         <f t="shared" ref="L3:L12" si="1" xml:space="preserve"> 924*POWER(K3,13) - 6006 * POWER(K3,12) + 16380 * POWER(K3,11) - 24024 * POWER(K3,10)  + 20020 * POWER(K3,9) - 9009 * POWER(K3,8) + 1716 * POWER(K3,7)</f>
         <v>9.9285486400000066E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="O3">
+        <v>14.4</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" ref="P3:P6" si="2">$P$1/O3*$H$2</f>
+        <v>208333.33333333334</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:Q6" si="3">$P$1/O3</f>
+        <v>347.22222222222223</v>
+      </c>
+      <c r="R3" s="3">
+        <f t="shared" ref="R3:R6" si="4">Q3/60</f>
+        <v>5.7870370370370372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -604,8 +657,23 @@
         <f t="shared" si="1"/>
         <v>7.0035611648000037E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="O4">
+        <v>20</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="2"/>
+        <v>150000</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="R4" s="3">
+        <f t="shared" si="4"/>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -629,8 +697,23 @@
         <f t="shared" si="1"/>
         <v>6.237521179919997E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="O5">
+        <v>24</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="2"/>
+        <v>125000</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="3"/>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="R5" s="3">
+        <f t="shared" si="4"/>
+        <v>3.4722222222222223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -655,8 +738,23 @@
         <f t="shared" si="1"/>
         <v>0.22884395253759982</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="2"/>
+        <v>100000</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="3"/>
+        <v>166.66666666666666</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" si="4"/>
+        <v>2.7777777777777777</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -688,7 +786,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -699,7 +797,7 @@
         <v>1.82</v>
       </c>
       <c r="D8">
-        <f>B8*C8*$H$2</f>
+        <f t="shared" ref="D8:D22" si="5">B8*C8*$H$2</f>
         <v>9.9372000000000007</v>
       </c>
       <c r="E8">
@@ -723,7 +821,7 @@
         <v>0.77115604746240507</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -734,19 +832,19 @@
         <v>3.6</v>
       </c>
       <c r="D9">
-        <f>B9*C9*$H$2</f>
+        <f t="shared" si="5"/>
         <v>18.468</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E21" si="2">B9*$H$2</f>
+        <f t="shared" ref="E9:E21" si="6">B9*$H$2</f>
         <v>5.13</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F22" si="3">1/E9*60</f>
+        <f t="shared" ref="F9:F22" si="7">1/E9*60</f>
         <v>11.695906432748538</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G22" si="4">1/E9</f>
+        <f t="shared" ref="G9:G22" si="8">1/E9</f>
         <v>0.19493177387914232</v>
       </c>
       <c r="I9" s="1"/>
@@ -757,8 +855,27 @@
         <f t="shared" si="1"/>
         <v>0.93762478820084993</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <f>N9*10</f>
+        <v>20</v>
+      </c>
+      <c r="P9" s="2">
+        <f>$P$1/O9*$H$2</f>
+        <v>150000</v>
+      </c>
+      <c r="Q9" s="2">
+        <f>$P$1/O9</f>
+        <v>250</v>
+      </c>
+      <c r="R9" s="3">
+        <f>Q9/60</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -769,19 +886,19 @@
         <v>2.88</v>
       </c>
       <c r="D10">
-        <f>B10*C10*$H$2</f>
+        <f t="shared" si="5"/>
         <v>14.428800000000001</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>5.01</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>11.976047904191617</v>
       </c>
       <c r="G10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.19960079840319361</v>
       </c>
       <c r="I10" s="1"/>
@@ -792,8 +909,25 @@
         <f t="shared" si="1"/>
         <v>0.99299643883495037</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="N10" s="3"/>
+      <c r="O10">
+        <f>N9*14.4</f>
+        <v>28.8</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" ref="P10:P13" si="9">$P$1/O10*$H$2</f>
+        <v>104166.66666666667</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" ref="Q10:Q13" si="10">$P$1/O10</f>
+        <v>173.61111111111111</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" ref="R10:R13" si="11">Q10/60</f>
+        <v>2.8935185185185186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -804,19 +938,19 @@
         <v>4.74</v>
       </c>
       <c r="D11">
-        <f>B11*C11*$H$2</f>
+        <f t="shared" si="5"/>
         <v>23.463000000000001</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.95</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>12.121212121212121</v>
       </c>
       <c r="G11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.20202020202020202</v>
       </c>
       <c r="I11" s="1"/>
@@ -827,8 +961,25 @@
         <f t="shared" si="1"/>
         <v>0.99990071451395579</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="N11" s="3"/>
+      <c r="O11">
+        <f>N9*20</f>
+        <v>40</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="9"/>
+        <v>75000</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="10"/>
+        <v>125</v>
+      </c>
+      <c r="R11" s="3">
+        <f t="shared" si="11"/>
+        <v>2.0833333333333335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -839,19 +990,19 @@
         <v>2.36</v>
       </c>
       <c r="D12">
-        <f>B12*C12*$H$2</f>
+        <f t="shared" si="5"/>
         <v>9.9827999999999992</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.2299999999999995</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>14.18439716312057</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.23640661938534283</v>
       </c>
       <c r="I12" s="1"/>
@@ -862,8 +1013,25 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="N12" s="3"/>
+      <c r="O12">
+        <f>N9*24</f>
+        <v>48</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="9"/>
+        <v>62500</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="10"/>
+        <v>104.16666666666667</v>
+      </c>
+      <c r="R12" s="3">
+        <f t="shared" si="11"/>
+        <v>1.7361111111111112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -874,24 +1042,41 @@
         <v>7.5</v>
       </c>
       <c r="D13">
-        <f>B13*C13*$H$2</f>
+        <f t="shared" si="5"/>
         <v>28.8</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.8400000000000003</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>15.624999999999998</v>
       </c>
       <c r="G13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.26041666666666663</v>
       </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="N13" s="3"/>
+      <c r="O13">
+        <f>N9*30</f>
+        <v>60</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="9"/>
+        <v>50000</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="10"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="R13" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3888888888888888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -902,24 +1087,24 @@
         <v>9.42</v>
       </c>
       <c r="D14">
-        <f>B14*C14*$H$2</f>
+        <f t="shared" si="5"/>
         <v>24.586199999999998</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2.61</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>22.988505747126439</v>
       </c>
       <c r="G14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.38314176245210729</v>
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -930,24 +1115,24 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D15">
-        <f>B15*C15*$H$2</f>
+        <f t="shared" si="5"/>
         <v>14.415599999999998</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.758</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>34.129692832764505</v>
       </c>
       <c r="G15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.56882821387940841</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -958,19 +1143,19 @@
         <v>22.2</v>
       </c>
       <c r="D16">
-        <f>B16*C16*$H$2</f>
+        <f t="shared" si="5"/>
         <v>25.973999999999997</v>
       </c>
       <c r="E16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.17</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>51.282051282051285</v>
       </c>
       <c r="G16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.85470085470085477</v>
       </c>
       <c r="I16" s="1"/>
@@ -986,19 +1171,19 @@
         <v>30</v>
       </c>
       <c r="D17">
-        <f>B17*C17*$H$2</f>
+        <f t="shared" si="5"/>
         <v>30.06</v>
       </c>
       <c r="E17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.002</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>59.880239520958078</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.99800399201596801</v>
       </c>
       <c r="I17" s="1"/>
@@ -1014,19 +1199,19 @@
         <v>19.739999999999998</v>
       </c>
       <c r="D18">
-        <f>B18*C18*$H$2</f>
+        <f t="shared" si="5"/>
         <v>17.884439999999998</v>
       </c>
       <c r="E18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.90600000000000003</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>66.225165562913901</v>
       </c>
       <c r="G18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1037527593818983</v>
       </c>
       <c r="I18" s="1"/>
@@ -1042,19 +1227,19 @@
         <v>32.11</v>
       </c>
       <c r="D19">
-        <f>B19*C19*$H$2</f>
+        <f t="shared" si="5"/>
         <v>26.9724</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.84</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>71.428571428571431</v>
       </c>
       <c r="G19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.1904761904761905</v>
       </c>
       <c r="I19" s="1"/>
@@ -1070,19 +1255,19 @@
         <v>44.44</v>
       </c>
       <c r="D20">
-        <f>B20*C20*$H$2</f>
+        <f t="shared" si="5"/>
         <v>29.863679999999995</v>
       </c>
       <c r="E20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.67199999999999993</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>89.285714285714306</v>
       </c>
       <c r="G20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.4880952380952384</v>
       </c>
     </row>
@@ -1097,19 +1282,19 @@
         <v>50</v>
       </c>
       <c r="D21">
-        <f>B21*C21*$H$2</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="E21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.54</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>111.1111111111111</v>
       </c>
       <c r="G21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1.8518518518518516</v>
       </c>
     </row>
@@ -1124,7 +1309,7 @@
         <v>1000</v>
       </c>
       <c r="D22">
-        <f>B22*C22*$H$2</f>
+        <f t="shared" si="5"/>
         <v>48</v>
       </c>
       <c r="E22">
@@ -1132,11 +1317,11 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1250</v>
       </c>
       <c r="G22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20.833333333333332</v>
       </c>
     </row>

</xml_diff>